<commit_message>
Add support for dithering MM/dd and MMMM yyyy patterns.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dates and times.xlsx
+++ b/DECS Excel Add-Ins/test files/dates and times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C829F5-6342-4F10-9000-3097323CFD0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B71B8D-FB21-4355-AF82-876524C37C3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{536CA7A3-242A-4ADD-BB44-BC599D1F36F8}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Note data</t>
   </si>
   <si>
-    <t>Patient X has an appointment on 1/2/2005 08:52 PM PST and another at 2/3/2006 09:53 PM PDT.</t>
-  </si>
-  <si>
-    <t>Can we see Patient X at 3/4/2007 11:00 AM PST and also at 4/5/2008 03:53 PM PDT?</t>
-  </si>
-  <si>
     <t>Nonsense</t>
   </si>
   <si>
@@ -61,6 +55,24 @@
   </si>
   <si>
     <t>nwronhwpwh</t>
+  </si>
+  <si>
+    <t>What about just June 1999?</t>
+  </si>
+  <si>
+    <t>ymuw64y7mu3w4e6</t>
+  </si>
+  <si>
+    <t>m75ir67i ,r7i68oi</t>
+  </si>
+  <si>
+    <t>Patient X has an appointment on 1/2/2005 08:52 PM PST and another at 12/3/2006 09:53 PM PDT.</t>
+  </si>
+  <si>
+    <t>Can we see Patient X at 3/14/2007 11:00 AM PST and also at 04/15/2008 03:53 PM PDT?</t>
+  </si>
+  <si>
+    <t>Let's try just month/day without year like 11/28 or 3/2 and so forth.</t>
   </si>
 </sst>
 </file>
@@ -424,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96721D22-1CCA-4806-98CF-158E0FCAF2D0}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,47 +453,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>